<commit_message>
discount rate for Times model
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\osemosys_India\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C4E687-C6B8-4804-8EEE-B917AB527BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECDB482-BBBA-4C8B-9CAD-F12A3E720E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTT" sheetId="16" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
   <si>
     <t>~BookRegions_Map</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>osemosys_default</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -8588,10 +8594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -8660,6 +8666,16 @@
         <v>106</v>
       </c>
     </row>
+    <row r="7" spans="1:11">
+      <c r="G7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="G8" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8672,7 +8688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B3:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>